<commit_message>
Added base text and data to include in web pages
</commit_message>
<xml_diff>
--- a/Documentation/Contribution.xlsx
+++ b/Documentation/Contribution.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c56e8f5f32bf7d06/Desktop/Napier/Group Project/git/MENS-SHED-SOC09109/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40435226\source\repos\JBLACK2889\MENS-SHED-SOC09109\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E78EB922-D658-4752-B819-C1381A7FA057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13425" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -74,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1102,21 +1101,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>2</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>3</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>5</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>6</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>7</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>8</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>10</v>
       </c>
@@ -1325,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>11</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>12</v>
       </c>
@@ -1361,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>13</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6">
         <v>45040</v>
@@ -1395,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6">
         <v>45047</v>
@@ -1411,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6">
         <v>45054</v>
@@ -1427,10 +1426,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
midpoint review and basic bcrypt intitialisation added
</commit_message>
<xml_diff>
--- a/Documentation/Contribution.xlsx
+++ b/Documentation/Contribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c56e8f5f32bf7d06/Desktop/Napier/Group Project/git/MENS-SHED-SOC09109/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jclok\GitHub\MENS-SHED-SOC09109\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_A2E12BE753F6E8702C0393533DA8353E5B136FDB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8912CD5-7440-4899-B6BC-63EAC82C79A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7259C191-1486-4D74-8AB3-31B0AFE9FCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,22 +719,22 @@
       <sheetData sheetId="2">
         <row r="9">
           <cell r="L9">
-            <v>0.84496124031007758</v>
+            <v>0.73154362416107388</v>
           </cell>
         </row>
         <row r="12">
           <cell r="L12">
-            <v>0</v>
+            <v>0.13422818791946309</v>
           </cell>
         </row>
         <row r="15">
           <cell r="L15">
-            <v>0.11627906976744186</v>
+            <v>0.10067114093959731</v>
           </cell>
         </row>
         <row r="18">
           <cell r="L18">
-            <v>3.875968992248062E-2</v>
+            <v>3.3557046979865772E-2</v>
           </cell>
         </row>
         <row r="21">
@@ -815,27 +815,27 @@
       <sheetData sheetId="5">
         <row r="9">
           <cell r="L9">
-            <v>0.21839080459770116</v>
+            <v>0.2</v>
           </cell>
         </row>
         <row r="12">
           <cell r="L12">
-            <v>9.1954022988505746E-2</v>
+            <v>0.16842105263157894</v>
           </cell>
         </row>
         <row r="15">
           <cell r="L15">
-            <v>0.28735632183908044</v>
+            <v>0.26315789473684209</v>
           </cell>
         </row>
         <row r="18">
           <cell r="L18">
-            <v>0.28735632183908044</v>
+            <v>0.26315789473684209</v>
           </cell>
         </row>
         <row r="21">
           <cell r="L21">
-            <v>0.11494252873563218</v>
+            <v>0.10526315789473684</v>
           </cell>
         </row>
         <row r="24">
@@ -847,12 +847,12 @@
       <sheetData sheetId="6">
         <row r="9">
           <cell r="L9">
-            <v>0.3902439024390244</v>
+            <v>0.35555555555555557</v>
           </cell>
         </row>
         <row r="12">
           <cell r="L12">
-            <v>0</v>
+            <v>8.8888888888888892E-2</v>
           </cell>
         </row>
         <row r="15">
@@ -862,7 +862,7 @@
         </row>
         <row r="18">
           <cell r="L18">
-            <v>0.6097560975609756</v>
+            <v>0.55555555555555558</v>
           </cell>
         </row>
         <row r="21">
@@ -879,12 +879,12 @@
       <sheetData sheetId="7">
         <row r="9">
           <cell r="L9">
-            <v>9.0909090909090912E-2</v>
+            <v>5.8823529411764705E-2</v>
           </cell>
         </row>
         <row r="12">
           <cell r="L12">
-            <v>0</v>
+            <v>0.35294117647058826</v>
           </cell>
         </row>
         <row r="15">
@@ -894,7 +894,7 @@
         </row>
         <row r="18">
           <cell r="L18">
-            <v>0.90909090909090906</v>
+            <v>0.58823529411764708</v>
           </cell>
         </row>
         <row r="21">
@@ -911,12 +911,12 @@
       <sheetData sheetId="8">
         <row r="9">
           <cell r="L9">
-            <v>1</v>
+            <v>0.79646017699115035</v>
           </cell>
         </row>
         <row r="12">
           <cell r="L12">
-            <v>0</v>
+            <v>0.20353982300884954</v>
           </cell>
         </row>
         <row r="15">
@@ -1398,17 +1398,17 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1470,11 +1470,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="2">
-        <f>SUM(C2:H2)</f>
+        <f t="shared" ref="J2:J16" si="0">SUM(C2:H2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1483,15 +1483,15 @@
       </c>
       <c r="C3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$9</f>
-        <v>0.84496124031007758</v>
+        <v>0.73154362416107388</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$15</f>
-        <v>0.11627906976744186</v>
+        <v>0.10067114093959731</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$12</f>
-        <v>0</v>
+        <v>0.13422818791946309</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$21</f>
@@ -1499,18 +1499,18 @@
       </c>
       <c r="G3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$18</f>
-        <v>3.875968992248062E-2</v>
+        <v>3.3557046979865772E-2</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]WK 2 23-01-23'!$L$24</f>
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <f>SUM(C3:H3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1542,11 +1542,11 @@
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <f>SUM(C4:H4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1578,11 +1578,11 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <f>SUM(C5:H5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1591,34 +1591,34 @@
       </c>
       <c r="C6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$9</f>
-        <v>0.21839080459770116</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$15</f>
-        <v>0.28735632183908044</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="E6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$12</f>
-        <v>9.1954022988505746E-2</v>
+        <v>0.16842105263157894</v>
       </c>
       <c r="F6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$21</f>
-        <v>0.11494252873563218</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="G6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$18</f>
-        <v>0.28735632183908044</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="H6" s="2">
         <f>'[1]WK 5 13-02-23'!$L$24</f>
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <f>SUM(C6:H6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="C7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$9</f>
-        <v>0.3902439024390244</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="D7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$15</f>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="E7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$12</f>
-        <v>0</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="F7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$21</f>
@@ -1643,18 +1643,18 @@
       </c>
       <c r="G7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$18</f>
-        <v>0.6097560975609756</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="H7" s="2">
         <f>'[1]WK 6 20-02-23 '!$L$24</f>
         <v>0</v>
       </c>
       <c r="J7" s="2">
-        <f>SUM(C7:H7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$9</f>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$15</f>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="E8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$12</f>
-        <v>0</v>
+        <v>0.35294117647058826</v>
       </c>
       <c r="F8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$21</f>
@@ -1679,18 +1679,18 @@
       </c>
       <c r="G8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$18</f>
-        <v>0.90909090909090906</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="H8" s="2">
         <f>'[1]WK 7 27-02-23'!$L$24</f>
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <f>SUM(C8:H8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="C9" s="2">
         <f>'[1]WK 8 06-03-23'!$L$9</f>
-        <v>1</v>
+        <v>0.79646017699115035</v>
       </c>
       <c r="D9" s="2">
         <f>'[1]WK 8 06-03-23'!$L$15</f>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="E9" s="2">
         <f>'[1]WK 8 06-03-23'!$L$12</f>
-        <v>0</v>
+        <v>0.20353982300884954</v>
       </c>
       <c r="F9" s="2">
         <f>'[1]WK 8 06-03-23'!$L$21</f>
@@ -1722,11 +1722,11 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <f>SUM(C9:H9)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1740,11 +1740,11 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="J10" s="2">
-        <f>SUM(C10:H10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1758,11 +1758,11 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="J11" s="2">
-        <f>SUM(C11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1776,11 +1776,11 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="J12" s="2">
-        <f>SUM(C12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1794,11 +1794,11 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="J13" s="2">
-        <f>SUM(C13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1812,11 +1812,11 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14" s="2">
-        <f>SUM(C14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1830,11 +1830,11 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="J15" s="2">
-        <f>SUM(C15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1848,11 +1848,11 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="J16" s="2">
-        <f>SUM(C16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1868,35 +1868,35 @@
         <v>45054</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="2">
-        <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.49452704253757318</v>
+        <f t="shared" ref="C20:H20" si="1">SUM(C2:C13)/COUNT(C2:C13)</f>
+        <v>0.44426177352052948</v>
       </c>
       <c r="D20" s="2">
-        <f>SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.11757542212391599</v>
+        <f t="shared" si="1"/>
+        <v>0.11259962763265563</v>
       </c>
       <c r="E20" s="2">
-        <f>SUM(E2:E13)/COUNT(E2:E13)</f>
-        <v>8.6339285542351957E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.19334742378370984</v>
       </c>
       <c r="F20" s="2">
-        <f>SUM(F2:F13)/COUNT(F2:F13)</f>
-        <v>3.4052855462032766E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2842934106920844E-2</v>
       </c>
       <c r="G20" s="2">
-        <f>SUM(G2:G13)/COUNT(G2:G13)</f>
-        <v>0.26750539433412612</v>
+        <f t="shared" si="1"/>
+        <v>0.2169482409561842</v>
       </c>
       <c r="H20" s="2">
-        <f>SUM(H2:H13)/COUNT(H2:H13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J20" s="2">

</xml_diff>